<commit_message>
excel export ready parte 1
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,14 +436,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>indice</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>codigo</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>codigo_sap</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>descripcion</t>
@@ -451,82 +451,92 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>marca</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>cantidad</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>precion sin igv</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>precio</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total_sin_igv</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A3</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>mouse</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
+      <c r="F2" t="n">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
+        <v>8.470000000000001</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A2</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>teclado</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
+          <t>mouse 32</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>celular</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="n">
+        <v>16.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>